<commit_message>
Change names of the categories
</commit_message>
<xml_diff>
--- a/autoimmune/R.GR.autoimmune/data/icd9_mapping.xlsx
+++ b/autoimmune/R.GR.autoimmune/data/icd9_mapping.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3603" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3603" uniqueCount="205">
   <si>
     <t>Kawasaki_disease</t>
   </si>
@@ -511,9 +511,6 @@
     <t>DOID:9352</t>
   </si>
   <si>
-    <t xml:space="preserve">Hematological_param </t>
-  </si>
-  <si>
     <t>metabolic</t>
   </si>
   <si>
@@ -632,6 +629,15 @@
   </si>
   <si>
     <t>Ankylosing spondylitis</t>
+  </si>
+  <si>
+    <t>neurologic</t>
+  </si>
+  <si>
+    <t>immunologic</t>
+  </si>
+  <si>
+    <t>hematologic</t>
   </si>
 </sst>
 </file>
@@ -51781,8 +51787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38:E39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39:E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -51827,137 +51833,137 @@
         <v>85</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>87</v>
+        <v>202</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="I2" s="5">
-        <v>995.3</v>
+        <v>55</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B3" s="2">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>87</v>
+        <v>202</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>140</v>
+        <v>72</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>160</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>165</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="B4" s="2">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>87</v>
+        <v>202</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>103</v>
+        <v>147</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>166</v>
+        <v>75</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2">
-        <v>522</v>
+        <v>63</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>163</v>
+        <v>202</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="B6" s="2">
-        <v>339</v>
+        <v>522</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>87</v>
+        <v>162</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>151</v>
+        <v>59</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>161</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>189</v>
@@ -51965,759 +51971,759 @@
     </row>
     <row r="7" spans="1:11" ht="15">
       <c r="A7" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7" s="2">
-        <v>175</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>86</v>
+        <v>197</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>162</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>136</v>
+        <v>53</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>157</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="2" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B8" s="2">
-        <v>74</v>
+        <v>430</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>86</v>
+        <v>162</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>197</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="2" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="B9" s="2">
-        <v>46</v>
+        <v>141</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>86</v>
+        <v>162</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>75</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:11" ht="15">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="B10" s="2">
-        <v>696</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>87</v>
+        <v>47</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>162</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="2" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B11" s="2">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>86</v>
+        <v>162</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>171</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:11" ht="15">
       <c r="A12" s="2" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2">
-        <v>56</v>
+        <v>331</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>87</v>
+        <v>162</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>172</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:11" ht="15">
       <c r="A13" s="2" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="B13" s="2">
-        <v>121</v>
+        <v>261</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>87</v>
+        <v>162</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>66</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:11" ht="15">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B14" s="2">
-        <v>787</v>
+        <v>173</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>87</v>
+        <v>162</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>173</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:11" ht="15">
       <c r="A15" s="2" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="B15" s="2">
-        <v>447</v>
+        <v>128</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>87</v>
+        <v>162</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>192</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:11" ht="15">
       <c r="A16" s="2" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B16" s="2">
-        <v>275</v>
+        <v>234</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>87</v>
+        <v>162</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>198</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2">
-        <v>80</v>
+        <v>192</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>87</v>
+        <v>162</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>193</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="I17" s="5"/>
     </row>
     <row r="18" spans="1:11" ht="15">
       <c r="A18" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B18" s="2">
-        <v>370</v>
+        <v>160</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>87</v>
+        <v>203</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>91</v>
+        <v>13</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="I18" s="5">
+        <v>995.3</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="2" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="B19" s="2">
-        <v>197</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>163</v>
+        <v>66</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>203</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>157</v>
+        <v>70</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>140</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>194</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B20" s="2">
-        <v>118</v>
+        <v>48</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>87</v>
+        <v>203</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>90</v>
+        <v>29</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>195</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15">
       <c r="A21" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B21" s="2">
-        <v>264</v>
+        <v>339</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>87</v>
+        <v>203</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>8</v>
+        <v>167</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>8</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="2" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="B22" s="2">
-        <v>66</v>
+        <v>696</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>87</v>
+        <v>203</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H22" s="13" t="s">
-        <v>154</v>
+        <v>9</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>144</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>180</v>
+        <v>10</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>199</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15">
       <c r="A23" s="2" t="s">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="B23" s="2">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>87</v>
+        <v>203</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>61</v>
+        <v>171</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>61</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15">
       <c r="A24" s="2" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="B24" s="2">
-        <v>221</v>
+        <v>121</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>87</v>
+        <v>203</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>181</v>
+        <v>66</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>181</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B25" s="2">
-        <v>43</v>
+        <v>787</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>87</v>
+        <v>203</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>150</v>
+        <v>25</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>142</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>200</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15">
       <c r="A26" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B26" s="2">
-        <v>195</v>
+        <v>447</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>87</v>
+        <v>203</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>12</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B27" s="2">
-        <v>236</v>
+        <v>275</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>87</v>
+        <v>203</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H27" s="13" t="s">
-        <v>156</v>
+        <v>17</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>145</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15">
       <c r="A28" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B28" s="2">
-        <v>207</v>
+        <v>80</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>87</v>
+        <v>203</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H28" s="11" t="s">
-        <v>137</v>
+        <v>31</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>159</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="2" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="B29" s="2">
-        <v>430</v>
+        <v>370</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>163</v>
+        <v>203</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I29" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="2" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="B30" s="2">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>163</v>
+        <v>203</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I30" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="2" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="B31" s="2">
-        <v>47</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>163</v>
+        <v>264</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>203</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I31" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="2" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="B32" s="2">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>163</v>
+        <v>203</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I32" s="5"/>
-    </row>
-    <row r="33" spans="1:9">
+        <v>64</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="2" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="B33" s="2">
-        <v>331</v>
+        <v>155</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>163</v>
+        <v>203</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I33" s="5"/>
-    </row>
-    <row r="34" spans="1:9">
+        <v>61</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="2" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="B34" s="2">
-        <v>261</v>
+        <v>221</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>163</v>
+        <v>203</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I34" s="5"/>
-    </row>
-    <row r="35" spans="1:9">
+        <v>2</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B35" s="2">
-        <v>173</v>
+        <v>43</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>163</v>
+        <v>203</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I35" s="5"/>
-    </row>
-    <row r="36" spans="1:9">
+        <v>15</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="2">
+        <v>195</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="2">
+        <v>236</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="2">
+        <v>207</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B39" s="2">
         <v>368</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="F36" s="2" t="s">
+      <c r="E39" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I36" s="6"/>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="2" t="s">
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B40" s="2">
         <v>299</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="F37" s="2" t="s">
+      <c r="E40" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I37" s="6"/>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B38" s="2">
-        <v>128</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I38" s="5"/>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" s="2">
-        <v>234</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I39" s="5"/>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B40" s="2">
-        <v>192</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I40" s="5"/>
+      <c r="I40" s="6"/>
     </row>
   </sheetData>
-  <sortState ref="A2:I40">
-    <sortCondition ref="I1"/>
+  <sortState ref="A2:K40">
+    <sortCondition descending="1" ref="E1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Reorganizing categories and names
</commit_message>
<xml_diff>
--- a/autoimmune/R.GR.autoimmune/data/icd9_mapping.xlsx
+++ b/autoimmune/R.GR.autoimmune/data/icd9_mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16440" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="icd9_mapping.txt" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3603" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3603" uniqueCount="223">
   <si>
     <t>Kawasaki_disease</t>
   </si>
@@ -637,7 +637,61 @@
     <t>immunologic</t>
   </si>
   <si>
-    <t>hematologic</t>
+    <t>other</t>
+  </si>
+  <si>
+    <t>C reactive protein</t>
+  </si>
+  <si>
+    <t>Platelet counts</t>
+  </si>
+  <si>
+    <t>Red blood cell traits</t>
+  </si>
+  <si>
+    <t>Alzheimers combined</t>
+  </si>
+  <si>
+    <t>Progressive supranuclear palsy</t>
+  </si>
+  <si>
+    <t>Restless legs syndrome</t>
+  </si>
+  <si>
+    <t>Chronic kidney disease</t>
+  </si>
+  <si>
+    <t>Fasting glucose related traits</t>
+  </si>
+  <si>
+    <t>HDL cholesterol</t>
+  </si>
+  <si>
+    <t>LDL cholesterol</t>
+  </si>
+  <si>
+    <t>Behcets disease</t>
+  </si>
+  <si>
+    <t>Multiple sclerosis</t>
+  </si>
+  <si>
+    <t>Kawasaki disease</t>
+  </si>
+  <si>
+    <t>Primary biliary cirrhosis</t>
+  </si>
+  <si>
+    <t>Primary sclerosing cholangitis</t>
+  </si>
+  <si>
+    <t>Atopic dermatitis</t>
+  </si>
+  <si>
+    <t>Rheumatoid arthritis</t>
+  </si>
+  <si>
+    <t>Renal function related traits</t>
   </si>
 </sst>
 </file>
@@ -51787,8 +51841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39:E40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -51839,887 +51893,887 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" ht="15">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B2" s="2">
-        <v>175</v>
+        <v>430</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>190</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="B3" s="2">
-        <v>74</v>
+        <v>141</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>196</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B4" s="2">
-        <v>46</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>202</v>
+        <v>47</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>204</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>75</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B5" s="2">
-        <v>63</v>
+        <v>128</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15">
+        <v>222</v>
+      </c>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="2" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2">
-        <v>522</v>
+        <v>192</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>162</v>
+        <v>204</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15">
+        <v>34</v>
+      </c>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B7" s="2">
-        <v>197</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>162</v>
+        <v>368</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>193</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B8" s="2">
-        <v>430</v>
+        <v>299</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>162</v>
+        <v>204</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" s="5"/>
+        <v>207</v>
+      </c>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="2" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B9" s="2">
-        <v>141</v>
+        <v>175</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>162</v>
+        <v>202</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:11" ht="15">
+        <v>208</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B10" s="2">
-        <v>47</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>162</v>
+        <v>74</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>202</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I10" s="5"/>
+        <v>209</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="2" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="B11" s="2">
-        <v>110</v>
+        <v>46</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>162</v>
+        <v>202</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="1:11" ht="15">
+        <v>210</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="2" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="B12" s="2">
-        <v>331</v>
+        <v>63</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>162</v>
+        <v>202</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:11" ht="15">
+        <v>62</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="2" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="B13" s="2">
-        <v>261</v>
+        <v>522</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>162</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="1:11" ht="15">
+        <v>60</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="2" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="B14" s="2">
-        <v>173</v>
-      </c>
-      <c r="E14" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E14" s="14" t="s">
         <v>162</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:11" ht="15">
+        <v>211</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B15" s="2">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>162</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>43</v>
+        <v>212</v>
       </c>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:11" ht="15">
+    <row r="16" spans="1:11">
       <c r="A16" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B16" s="2">
-        <v>234</v>
+        <v>331</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>162</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>41</v>
+        <v>213</v>
       </c>
       <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B17" s="2">
-        <v>192</v>
+        <v>261</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>162</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>33</v>
+        <v>214</v>
       </c>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="1:11" ht="15">
+    <row r="18" spans="1:11">
       <c r="A18" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B18" s="2">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>203</v>
+        <v>162</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="I18" s="5">
-        <v>995.3</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>195</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="2" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="B19" s="2">
-        <v>66</v>
+        <v>234</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>203</v>
+        <v>162</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H19" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="15">
+        <v>41</v>
+      </c>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B20" s="2">
-        <v>48</v>
+        <v>160</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>103</v>
+        <v>185</v>
+      </c>
+      <c r="I20" s="5">
+        <v>995.3</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>30</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15">
       <c r="A21" s="2" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="B21" s="2">
-        <v>339</v>
+        <v>66</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>151</v>
+        <v>215</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>140</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15">
       <c r="A22" s="2" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B22" s="2">
-        <v>696</v>
+        <v>48</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>93</v>
+        <v>30</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>10</v>
+        <v>165</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15">
       <c r="A23" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B23" s="2">
-        <v>56</v>
+        <v>339</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15">
       <c r="A24" s="2" t="s">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="B24" s="2">
-        <v>121</v>
+        <v>696</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>66</v>
+        <v>216</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15">
       <c r="A25" s="2" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="B25" s="2">
-        <v>787</v>
+        <v>56</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>25</v>
+        <v>217</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15">
       <c r="A26" s="2" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B26" s="2">
-        <v>447</v>
+        <v>121</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>173</v>
+        <v>66</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15">
       <c r="A27" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B27" s="2">
-        <v>275</v>
+        <v>787</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="15">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="2" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="B28" s="2">
-        <v>80</v>
+        <v>447</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>159</v>
+        <v>7</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>152</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15">
       <c r="A29" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B29" s="2">
-        <v>370</v>
+        <v>275</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>4</v>
+        <v>218</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15">
       <c r="A30" s="2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B30" s="2">
-        <v>118</v>
+        <v>80</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H30" s="11" t="s">
-        <v>139</v>
+        <v>219</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>159</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15">
       <c r="A31" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B31" s="2">
-        <v>264</v>
+        <v>370</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>8</v>
+        <v>176</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>8</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="2" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="B32" s="2">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H32" s="13" t="s">
-        <v>154</v>
+        <v>220</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>139</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15">
       <c r="A33" s="2" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="B33" s="2">
-        <v>155</v>
+        <v>264</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15">
       <c r="A34" s="2" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="B34" s="2">
-        <v>221</v>
+        <v>66</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H34" s="11" t="s">
-        <v>149</v>
+        <v>65</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>154</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="2" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="B35" s="2">
-        <v>43</v>
+        <v>155</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H35" s="12" t="s">
-        <v>150</v>
+        <v>61</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>153</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>181</v>
+        <v>61</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15">
       <c r="A36" s="2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B36" s="2">
-        <v>195</v>
+        <v>221</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>12</v>
+        <v>180</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B37" s="2">
-        <v>236</v>
+        <v>43</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H37" s="13" t="s">
-        <v>156</v>
+        <v>16</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>150</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15">
       <c r="A38" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B38" s="2">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>23</v>
+        <v>221</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>201</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="2" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="B39" s="2">
-        <v>368</v>
+        <v>236</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I39" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="2" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="B40" s="2">
-        <v>299</v>
+        <v>207</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I40" s="6"/>
+        <v>201</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>201</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:K40">

</xml_diff>

<commit_message>
Add ICD9 codes from AR FinalPhenotype_new.txt file
</commit_message>
<xml_diff>
--- a/autoimmune/R.GR.autoimmune/data/icd9_mapping.xlsx
+++ b/autoimmune/R.GR.autoimmune/data/icd9_mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16380" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="icd9_mapping.txt" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3603" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3742" uniqueCount="306">
   <si>
     <t>Kawasaki_disease</t>
   </si>
@@ -693,6 +693,255 @@
   <si>
     <t>Renal function related traits</t>
   </si>
+  <si>
+    <t>Disease Summary Name</t>
+  </si>
+  <si>
+    <t>General System</t>
+  </si>
+  <si>
+    <t>Applicable Gender</t>
+  </si>
+  <si>
+    <t>Monogenic Inheritance</t>
+  </si>
+  <si>
+    <t>ICD9 Codes</t>
+  </si>
+  <si>
+    <t>ICD9 Strings</t>
+  </si>
+  <si>
+    <t>Alzheimers_Disease</t>
+  </si>
+  <si>
+    <t>Neuropsychiatric</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>290.10|290.11|290.12|290.13|331.0|331.00|290.1</t>
+  </si>
+  <si>
+    <t>Alzheimer's disease **|"Presenile dementia, uncomplicated"|"Alzheimer's disease"|"Presenile dementia with delusional features"|"Presenile dementia with depressive features"|"Presenile dementia"|"Presenile dementia with delirium"</t>
+  </si>
+  <si>
+    <t>Extrapyramidal_Abnormal_Movement_Disorders</t>
+  </si>
+  <si>
+    <t>CNS</t>
+  </si>
+  <si>
+    <t>333.72|333.84|333.9|333.5|333.2|333.3|333.0|333.1|333.90|333.91|333.93|333.94|333.71|333.89|333.99|333.85|333.79|333.83|333.82|333.81</t>
+  </si>
+  <si>
+    <t>Acute dystonia due to drugs|"Blepharospasm"|"Essential and other specified forms of tremor"|"Other acquired torsion dystonia"|"Organic writers' cramp"|"Other and unspecified extrapyramidal diseases and abnormal movement disorders"|"Myoclonus"|"Spasmodic torticollis"|"Orofacial dyskinesia"|"Athetoid cerebral palsy"|"Other fragments of torsion dystonia"|"Subacute dyskinesia due to drugs"|"Benign shuddering attacks"|"Restless legs syndrome (RLS)"|"Other degenerative diseases of the basal ganglia"|"Tics of organic origin"|"Stiff_man syndrome"|"Unspecified extrapyramidal disease and abnormal movement disorder"|"Other choreas"|"Other extrapyramidal diseases and abnormal movement disorders"</t>
+  </si>
+  <si>
+    <t>346.2|346.3|346.0|346.1|339.0|346.7|346.5|346.8|346.9|346.90|346.91|346.92|346.93|346.10|346.11|346.12|346.13|346.52|346.50|346.51|346|346.53|346.72|346.73|346.70|346.71|346.32|346.33|346.30|346.31|346.83|346.82|346.81|346.80|346.03|346.02|346.01|346.00|339.04|339.01|339.00|339.03|339.02|346.21|346.20|346.23|346.22|346.43|346.42|346.41|346.40</t>
+  </si>
+  <si>
+    <t>Hemiplegic migraine|"Migraine without aura, with intractable migraine, so stated, without mention of status migrainosus"|"Migraine without aura"|"Other forms of migraine, with intractable migraine, so stated, without mention of status migrainosus"|"Migraine with aura, without mention of intractable migraine without mention of status migrainosus"|"Migraine, unspecified, without mention of intractable migraine without mention of status migrainosus"|"Menstrual migraine, without mention of intractable migraine with status migrainosus"|"Migraine, unspecified, without mention of intractable migraine with status migrainosus"|"Variants of migraine, not elsewhere classified"|"Persistent migraine aura without cerebral infarction, without mention of intractable migraine without mention of status migrainosus"|"Persistent migraine aura without cerebral infarction"|"Episodic paroxysmal hemicrania"|"Persistent migraine aura without cerebral infarction, with intractable migraine, so stated, without mention of status migrainosus"|"Persistent migraine aura without cerebral infarction, without mention of intractable migraine with status migrainosus"|"Chronic cluster headache"|"Migraine with aura, without mention of intractable migraine with status migrainosus"|"Episodic cluster headache"|"Hemiplegic migraine, without mention of intractable migraine without mention of status migrainosus"|"Migraine"|"Chronic paroxysmal hemicrania"|"Migraine, unspecified, with intractable migraine, so stated, with status migrainosus"|"Migraine with aura, with intractable migraine, so stated, without mention of status migrainosus"|"Migraine, unspecified, with intractable migraine, so stated, without mention of status migrainosus"|"Migraine, unspecified"|"Cluster headache syndrome, unspecified"|"Hemiplegic migraine, without mention of intractable migraine with status migrainosus"|"Persistent migraine aura without cerebral infarction, with intractable migraine, so stated, with status migrainosus"|"Chronic migraine without aura, with intractable migraine, so stated, without mention of status migrainosus"|"Hemiplegic migraine, with intractable migraine, so stated, with status migrainosus"|"Chronic migraine without aura, without mention of intractable migraine without mention of status migrainosus"|"Chronic migraine without aura, without mention of intractable migraine with status migrainosus"|"Migraine without aura, without mention of intractable migraine without mention of status migrainosus"|"Hemiplegic migraine, with intractable migraine, so stated, without mention of status migrainosus"|"Migraine without aura, without mention of intractable migraine with status migrainosus"|"Migraine with aura, with intractable migraine, so stated, with status migrainosus"|"Other forms of migraine"|"Variants of migraine, not elsewhere classified, with intractable migraine, so stated, without mention of status migrainosus"|"Other forms of migraine, without mention of intractable migraine without mention of status migrainosus"|"Migraine with aura"|"Variants of migraine, not elsewhere classified, without mention of intractable migraine without mention of status migrainosus"|"Chronic migraine without aura"|"Chronic migraine without aura, with intractable migraine, so stated, with status migrainosus"|"Variants of migraine, not elsewhere classified, without mention of intractable migraine with status migrainosus"|"Other forms of migraine, with intractable migraine, so stated, with status migrainosus"|"Menstrual migraine, with intractable migraine, so stated, without mention of status migrainosus"|"Variants of migraine, not elsewhere classified, with intractable migraine, so stated, with status migrainosus"|"Cluster headaches and other trigeminal autonomic cephalgias"|"Menstrual migraine, without mention of intractable migraine without mention of status migrainosus"|"Menstrual migraine, with intractable migraine, so stated, with status migrainosus"|"Migraine without aura, with intractable migraine, so stated, with status migrainosus"|"Other forms of migraine, without mention of intractable migraine with status migrainosus"</t>
+  </si>
+  <si>
+    <t>Type_II_Diabetes_Mellitus</t>
+  </si>
+  <si>
+    <t>Endocrine</t>
+  </si>
+  <si>
+    <t>250.32|250.20|250.30|250.22|250.42|250.40|250.02|250.00|250.10|250.12|250.82|250.80|250.90|250.92|250.50|250.52|250.72|250.60|250.70|250.62</t>
+  </si>
+  <si>
+    <t>Diabetes mellitus with other coma, type II [non_insulin dependent type] [NIDDM type] [adult_onset type] or unspecified type, uncontrolled|"type II diabetes mellitus [non_insulin dependent type] [NIDDM type] [adult_onset type] or unspecified type, not stated as uncontrolled, with ketoacidosis"|"Diabetes mellitus type II [non_insulin dependent type] [NIDDM type] [adult_onset type] or unspecified type, uncontrolled, with ophthalmic manifestations"|"Diabetes mellitus type II [non_insulin dependent type] [NIDDM type] [adult_onset type] or unspecified type, uncontrolled, with renal manifestations"|"Diabetes mellitus type II [non_insulin dependent type] [NIDDM type] [adult_onset type] or unspecified type, not stated as uncontrolled, with other specified manifestations"|"Diabetes mellitus, type II [non_insulin dependent type] [NIDDM type] [adult_onset type] or unspecified type, not stated as uncontrolled"|"type II diabetes mellitus [non_insulin dependent type] [NIDDM type] [adult_onset type] or unspecified type, uncontrolled, with ketoacidosis"|"Diabetes mellitus type II [non_insulin dependent type] [NIDDM type] [adult_onset type] or unspecified type, not stated as uncontrolled, with unspecified complication"|"Diabetes mellitus, type II [non_insulin dependent type] [NIDDM type] [adult_onset type] or unspecified type with hyperosmolarity, not stated as uncontrolled"|"Diabetes mellitus type II [non_insulin dependent type] [NIDDM type] [adult_onset type] or unspecified type, uncontrolled, with neurological manifestations"|"type II diabetes mellitus [non_insulin dependent type] [NIDDM type] [adult_onset type] or unspecified type, not stated as uncontrolled, without mention of complication"|"Diabetes mellitus type II [non_insulin dependent type] [NIDDM type] [adult_onset type] or unspecified type, not stated as uncontrolled, with renal manifestations"|"Diabetes mellitus type II [non_insulin dependent type] [NIDDM type] [adult_onset type] or unspecified type, uncontrolled, with peripheral circulatory disorders"|"Diabetes mellitus type II [non_insulin dependent type] [NIDDM type] [adult_onset type] or unspecified type, uncontrolled, with unspecified complication"|"Diabetes mellitus type II [non_insulin dependent type] [NIDDM type] [adult_onset type] or unspecified type, not stated as uncontrolled, with peripheral circulatory disorders"|"Diabetes mellitus type II [non_insulin dependent type] [NIDDM type] [adult_onset type] or unspecified type, uncontrolled, with other specified manifestations"|"Diabetes mellitustype II [non_insulin dependent type] [NIDDM type] [adult_onset type] or unspecified type with hyperosmolarity, uncontrolled"|"Diabetes mellitus type II [non_insulin dependent type] [NIDDM type] [adult_onset type] or unspecified type, not stated as uncontrolled, with ophthalmic manifestations"|"type II diabetes mellitus [non_insulin dependent type] [NIDDM type] [adult_onset type] or unspecified type, uncontrolled, without mention of complication"|"Diabetes mellitus type II [non_insulin dependent type] [NIDDM type] [adult_onset type] or unspecified type, not stated as uncontrolled, with neurological manifestations"</t>
+  </si>
+  <si>
+    <t>Chronic_Kidney_Disease</t>
+  </si>
+  <si>
+    <t>Urinary</t>
+  </si>
+  <si>
+    <t>586|586.0|584|585|588.0|585.1|585.9|585.6|585.5|585.4|585.3|585.2|588.81|585.0</t>
+  </si>
+  <si>
+    <t>Renal failure unspecified|"Secondary hyperparathyroidism (of renal origin)"|"Chronic kidney disease, Stage V"|"Chronic kidney disease (CKD) **"|"Chronic kidney disease, Stage III (moderate)"|"Renal failure unspecified **"|"Renal osteodystrophy"|"Chronic kidney disease, unspecified"|"Chronic kidney disease, Stage IV (severe)"|"Chronic kidney disease, Stage I"|"Chronic kidney disease, Stage II (mild)"|"Acute renal failure"|"End stage renal disease"|"Chronic kidney disease (CKD)"</t>
+  </si>
+  <si>
+    <t>Food_Allergy</t>
+  </si>
+  <si>
+    <t>Immune</t>
+  </si>
+  <si>
+    <t>477.1|558.3|693.1|692.5</t>
+  </si>
+  <si>
+    <t>Contact dermatitis and other eczema due to food in contact with skin|"Allergic rhinitis due to food"|"Allergic gastroenteritis and colitis"|"Dermatitis due to food taken internally"</t>
+  </si>
+  <si>
+    <t>Behcets_Syndrome</t>
+  </si>
+  <si>
+    <t>733.01|711.29|711.28|711.25|711.2|711.27|711.26|711.21|711.20|711.23|711.22|136.1|711.24</t>
+  </si>
+  <si>
+    <t>Arthropathy in Behcet's syndrome involving multiple sites|"Arthropathy in Behcet's syndrome involving forearm"|"Arthropathy in Behcet's syndrome involving other specified sites"|"Arthropathy in Behcet's syndrome involving ankle and foot"|"Behcet's syndrome"|"Arthropathy in Behcet's syndrome, site unspecified"|"Arthropathy in Behcet's syndrome"|"Senile osteoporosis"|"Arthropathy in Behcet's syndrome involving lower leg"|"Arthropathy in Behcet's syndrome involving shoulder region"|"Arthropathy in Behcet's syndrome involving upper arm"|"Arthropathy in Behcet's syndrome involving hand"|"Arthropathy in Behcet's syndrome involving pelvic region and thigh"</t>
+  </si>
+  <si>
+    <t>Thyroiditis</t>
+  </si>
+  <si>
+    <t>245.0|246.2|245|245.1|245.2|245.3|245.4|245.8|245.9</t>
+  </si>
+  <si>
+    <t>Thyroiditis|"Cyst of thyroid"|"Chronic fibrous thyroiditis"|"Other and unspecified chronic thyroiditis"|"Subacute thyroiditis"|"Iatrogenic thyroiditis"|"Chronic lymphocytic thyroiditis"|"Thyroiditis NOS"|"Acute thyroiditis"</t>
+  </si>
+  <si>
+    <t>Type_I_Diabetes_Mellitus</t>
+  </si>
+  <si>
+    <t>250.21|250.33|250.23|250.31|250.43|250.41|250.03|250.01|250.11|250.13|250.83|250.81|250.91|250.93|250.51|250.53|250.61|250.73|250.63|250.71</t>
+  </si>
+  <si>
+    <t>Diabetes mellitus type I [juvenile type], uncontrolled, with neurological manifestations|"Diabetes mellitus type I [insulin dependent type] [IDDM] [juvenile type], not stated as uncontrolled, with ophthalmic manifestations"|"Diabetes mellitus, type I [juvenile type] with hyperosmolarity, uncontrolled"|"Diabetes mellitus, type I [insulin dependent type] [IDDM] [juvenile type], not stated as uncontrolled"|"Diabetes mellitus type I [insulin dependent type] [IDDM] [juvenile type], uncontrolled, with unspecified complication"|"Diabetes mellitus type I [insulin dependent type] [IDDM] [juvenile type], not stated as uncontrolled, with renal manifestations"|"Diabetes mellitus type I [insulin dependent type] [IDDM] [juvenile type], not stated as uncontrolled, with peripheral circulatory disorders"|"type I diabetes mellitus [insulin dependent type] [IDDM] [juvenile type], not stated as uncontrolled, with ketoacidosis"|"Diabetes mellitus type I [insulin dependent type] [IDDM] [juvenile type], not stated as uncontrolled, with unspecified complication"|"Diabetes mellitus type I [juvenile type], uncontrolled, with other specified manifestations"|"Diabetes mellitus, type I [insulin dependent type] [IDDM] [juvenile type] with hyperosmolarity, not stated as uncontrolled"|"type I diabetes mellitus [juvenile type], uncontrolled, without mention of complication"|"type I diabetes mellitus [insulin dependent type] [IDDM] [juvenile type], not stated as uncontrolled, without mention of complication"|"Diabetes mellitus type I [juvenile type], uncontrolled, with renal manifestations"|"Diabetes mellitus type I [insulin dependent type] [IDDM] [juvenile type], not stated as uncontrolled, with neurological manifestations"|"Diabetes mellitus with other coma, type I [juvenile type], uncontrolled"|"type I diabetes mellitus [juvenile type], uncontrolled, with ketoacidosis"|"Diabetes mellitus type I [juvenile type], uncontrolled, with ophthalmic manifestations"|"Diabetes mellitus type I [insulin dependent type] [IDDM] [juvenile type], not stated as uncontrolled, with other specified manifestations"|"Diabetes mellitus type I [juvenile type], uncontrolled, with peripheral circulatory disorders"</t>
+  </si>
+  <si>
+    <t>Multiple_Sclerosis_Other_Demyelinating_Disease</t>
+  </si>
+  <si>
+    <t>341.1|341.0|340|341.9</t>
+  </si>
+  <si>
+    <t>Demyelinating disease of central nervous system, unspecified|"Neuromyelitis optica"|"Schilder's disease"|"Multiple sclerosis"</t>
+  </si>
+  <si>
+    <t>Kawasaki_Disease</t>
+  </si>
+  <si>
+    <t>Acute febrile mucocutaneous lymph node syndrome [MCLS]</t>
+  </si>
+  <si>
+    <t>493.22|493.20|493.90|493.91|493.12|493.11|493.10|493.00|493.01|493.02|493.92|493.9|493.8|493.81|493.82|493.2|493.1|493.0|493.21|493</t>
+  </si>
+  <si>
+    <t>Intrinsic asthma with acute exacerbation|"Extrinsic asthma with acute exacerbation"|"Extrinsic asthma with status asthmaticus"|"Chronic obstructive asthma, without mention of status asthmaticus"|"Exercise induced bronchospasm"|"Asthma, unspecified type, with acute exacerbation"|"Chronic obstructive asthma, with acute exacerbation"|"Intrinsic asthma with status asthmaticus"|"Asthma, unspecified type, without mention of status asthmaticus"|"Asthma"|"Extrinsic asthma"|"Intrinsic asthma"|"Intrinsic asthma without mention of status asthmaticus"|"Other forms of asthma"|"Extrinsic asthma without mention of status asthmaticus"|"Chronic obstructive asthma"|"Asthma, unspecified"|"Cough variant asthma"|"Asthma, unspecified type, with status asthmaticus"|"Chronic obstructive asthma, with status asthmaticus"</t>
+  </si>
+  <si>
+    <t>IBS_Crohns_Disease</t>
+  </si>
+  <si>
+    <t>555.0|555.1|555.2|564.1|555.9</t>
+  </si>
+  <si>
+    <t>Regional enteritis of small intestine|"Regional enteritis of large intestine"|"Regional enteritis of unspecified site"|"Irritable bowel syndrome"|"Regional enteritis of small intestine with large intestine"</t>
+  </si>
+  <si>
+    <t>Ulcerative_Colitis</t>
+  </si>
+  <si>
+    <t>556|556.6|556.5|556.4|556.3|556.2|556.1|556.0|556.9|556.8</t>
+  </si>
+  <si>
+    <t>Ulcerative (chronic) enterocolitis|"Other ulcerative colitis"|"Pseudopolyposis of colon"|"Ulcerative (chronic) proctosigmoiditis"|"Left_sided ulcerative (chronic) colitis"|"Ulcerative colitis, unspecified"|"Ulcerative (chronic) proctitis"|"Universal ulcerative (chronic) colitis"|"Ulcerative colitis"|"Ulcerative (chronic) ileocolitis"</t>
+  </si>
+  <si>
+    <t>Chronic_Liver_Disease</t>
+  </si>
+  <si>
+    <t>Hepatic</t>
+  </si>
+  <si>
+    <t>572.4|571.8|571.9|572.1|572.0|572.2|572|571|572.8|571.5</t>
+  </si>
+  <si>
+    <t>Hepatorenal syndrome|"Unspecified chronic liver disease without mention of alcohol"|"Portal pyemia"|"Chronic liver disease and cirrhosis"|"Cirrhosis of liver without mention of alcohol"|"Other sequelae of chronic liver disease"|"Liver abscess and sequelae of chronic liver disease"|"Other chronic nonalcoholic liver disease"|"Abscess of liver"|"Hepatic encephalopathy"</t>
+  </si>
+  <si>
+    <t>Biliary_Tract_Disease</t>
+  </si>
+  <si>
+    <t>595.4|574.91|574.90|575.2|574.7|595.8|595.9|575|574|575.1|575.0|575.5|574.3|574.70|574.9|574.8|575.8|575.9|575.6|574.2|574.1|574.0|571.6|574.6|574.5|574.4|576.9|575.10|574.20|574.21|575.11|576.1|576.0|576.3|576.2|574.00|574.01|576.8|576.4|574.80|574.81|574.40|574.41|575.12|574.60|574.61|575.3|595.89|576.5|032.84|574.31|574.30|576|574.51|574.50|574.11|574.10|575.4|574.71</t>
+  </si>
+  <si>
+    <t>Calculus of gallbladder without mention of cholecystitis, without mention of obstruction|"Perforation of gallbladder"|"Calculus of gallbladder and bile duct without cholecystitis, without mention of obstruction"|"Calculus of gallbladder and bile duct with acute cholecystitis"|"Calculus of gallbladder and bile duct with acute cholecystitis, without mention of obstruction"|"Calculus of gallbladder and bile duct without cholecystitis, with obstruction"|"Spasm of sphincter of Oddi"|"Calculus of gallbladder and bile duct with acute and chronic cholecystitis, with obstruction"|"Obstruction of gallbladder"|"Chronic cholecystitis"|"Calculus of bile duct without mention of cholecystitis, with obstruction"|"Calculus of gallbladder and bile duct with other cholecystitis, with obstruction"|"Calculus of gallbladder and bile duct with other cholecystitis"|"Calculus of gallbladder with other cholecystitis, with obstruction"|"Calculus of gallbladder with other cholecystitis, without mention of obstruction"|"Diphtheritic cystitis"|"Fistula of gallbladder"|"Perforation of bile duct"|"Calculus of gallbladder and bile duct with acute and chronic cholecystitis, without mention of obstruction"|"Other cholecystitis"|"Calculus of bile duct with acute cholecystitis"|"Calculus of bile duct with other cholecystitis, with obstruction"|"Hydrops of gallbladder"|"Calculus of bile duct with other cholecystitis, without mention of obstruction"|"Acute and chronic cholecystitis"|"Unspecified disorder of gallbladder"|"Cystitis NOS"|"Other specified disorders of gallbladder"|"Calculus of bile duct without mention of cholecystitis"|"Calculus of gallbladder without mention of cholecystitis"|"Fistula of bile duct"|"Other specified disorders of biliary tract"|"Calculus of gallbladder with acute cholecystitis, without mention of obstruction"|"Calculus of gallbladder and bile duct with acute cholecystitis, with obstruction"|"Calculus of gallbladder with acute cholecystitis"|"Other disorders of biliary tract"|"Biliary cirrhosis"|"Postcholecystectomy syndrome"|"Calculus of bile duct with acute cholecystitis, with obstruction"|"Calculus of gallbladder with acute cholecystitis, with obstruction"|"Cystitis in diseases classified elsewhere"|"Calculus of gallbladder without mention of cholecystitis, with obstruction"|"Calculus of bile duct with other cholecystitis"|"Cholecystitis NOS"|"Calculus of gallbladder and bile duct without cholecystitis"|"Calculus of bile duct with acute cholecystitis without mention of obstruction"|"Calculus of gallbladder with other cholecystitis"|"Calculus of gallbladder and bile duct with other cholecystitis, without mention of obstruction"|"Cholelithiasis"|"Cholesterolosis of gallbladder"|"Obstruction of bile duct"|"Acute cholecystitis"|"Calculus of gallbladder and bile duct with acute and chronic cholecystitis"|"Other specified types of cystitis"|"Cholangitis"|"Calculus of bile duct without mention of cholecystitis, without mention of obstruction"|"Other disorders of gallbladder"|"Unspecified disorder of biliary tract"</t>
+  </si>
+  <si>
+    <t>Celiac_Disease</t>
+  </si>
+  <si>
+    <t>Atopic_Contact_Dermatitis</t>
+  </si>
+  <si>
+    <t>708.4|708.5|708|708.1|708.2|708.3|708.8|708.9|708.0|692|693|691|692.81|692.83|692.84|692.89|373.32|691.8|693.9|692.0|692.1|692.2|692.3|692.4|693.8|692.6|692.8|692.9|693.0</t>
+  </si>
+  <si>
+    <t>Contact dermatitis and other eczema due to animal (cat) (dog) dander|"Dermatographic urticaria"|"Urticaria due to cold and heat"|"Dermatitis due to substances taken internally"|"Allergic urticaria"|"Atopic dermatitis and related conditions"|"Contact dermatitis and other eczema due to other specified agents"|"Dermatitis due to cosmetics"|"Cholinergic urticaria"|"Unspecified urticaria"|"Contact dermatitis and other eczema due to other chemical products"|"Contact dermatitis and other eczema due to solvents"|"Dermatitis due to unspecified substance taken internally"|"Dermatitis due to metals"|"Other atopic dermatitis"|"Contact dermatitis and other eczema due to drugs and medicines in contact with skin"|"Contact and allergic dermatitis of eyelid"|"Other specified urticaria"|"Contact dermatitis and other eczema due to oils and greases"|"Vibratory urticaria"|"Idiopathic urticaria"|"Contact dermatitis and other eczema due to plants [except food]"|"Contact dermatitis and other eczema due to detergents"|"Dermatitis due to other specified substances taken internally"|"Urticaria"|"Dermatitis due to drugs and medicines taken internally"|"Contact dermatitis and other eczema"|"Contact dermatitis and other eczema, unspecified cause"</t>
+  </si>
+  <si>
+    <t>Psoriasis_Related_Disorders</t>
+  </si>
+  <si>
+    <t>696.4|696.5|696|696.1|696.2|696.3|696.8|696.0</t>
+  </si>
+  <si>
+    <t>Other psoriasis and similar disorders|"Parapsoriasis"|"Pityriasis rosea"|"Psoriasis and similar disorders"|"Psoriatic arthropathy"|"Pityriasis rubra pilaris"|"Other and unspecified pityriasis"|"Other psoriasis and similar disorders excluding psoriatic arthropathy"</t>
+  </si>
+  <si>
+    <t>Integumentary</t>
+  </si>
+  <si>
+    <t>704.0|704.00|704.02|704.01|704.09</t>
+  </si>
+  <si>
+    <t>Alopecia NOS|"Alopecia areata"|"Telogen effluvium"|"Other alopecia"|"Alopecia"</t>
+  </si>
+  <si>
+    <t>Dyschromia</t>
+  </si>
+  <si>
+    <t>709.0|709.00|709.01|709.09</t>
+  </si>
+  <si>
+    <t>Dyschromia|"Other dyschromia"|"Dyschromia, unspecified"|"Vitiligo"</t>
+  </si>
+  <si>
+    <t>Lupus_Erythematosus</t>
+  </si>
+  <si>
+    <t>710.0|373.34|695.4</t>
+  </si>
+  <si>
+    <t>Systemic lupus erythematosus|"Discoid lupus erythematosus of eyelid"|"Lupus erythematosus"</t>
+  </si>
+  <si>
+    <t>Non_Specific_Skin_Disorder</t>
+  </si>
+  <si>
+    <t>709.1|707.00|707.02|707.03|707.04|707.05|707.06|707.01|709.9|707.09|707|701|702|707.25|707.2|707.1|707.0|707.22|707.8|707.9|707.23|706.8|707.20|702.8|705.2|706.2|707.07|701.9|701.8|709.3|709.8|701.1|701.0|701.3|701.2|701.4|707.24|707.19|707.15|707.14|707.13|707.12|707.11|710|705.21|705.22|707.21|707.10|710.9|710.8|709|695.9|709.2</t>
+  </si>
+  <si>
+    <t>Pressure ulcer|"Decubitus ulcer, buttock"|"Decubitus ulcer, ankle"|"Decubitus ulcer, unspecified site"|"Unspecified diffuse connective tissue disease"|"Keloid scar"|"Chronic ulcer of unspecified site"|"Pressure ulcer stage IV"|"Decubitus ulcer, upper back"|"Ulcer of calf"|"Pressure ulcer, unspecified stage"|"Pressure ulcer stage I"|"Ulcer of ankle"|"Diffuse diseases of connective tissue"|"Decubitus ulcer, heel"|"Ulcer of other part of lower limb"|"Pressure ulcer stages"|"Unspecified hypertrophic and atrophic conditions of skin"|"Ulcer of other part of foot"|"Decubitus ulcer, other site"|"Unspecified disorder of skin and subcutaneous tissue"|"Acquired acanthosis nigricans"|"Other hypertrophic and atrophic conditions of skin"|"Ulcer of lower limb, unspecified"|"Primary focal hyperhidrosis"|"Other specified disorders of skin"|"Decubitus ulcer, elbow"|"Pressure ulcer stage II"|"Other specified diffuse diseases of connective tissue"|"Ulcer of heel and midfoot"|"Chronic ulcer of skin"|"Pressure ulcer stage III"|"Ulcer of thigh"|"Pressure ulcer, unstageable"|"Focal hyperhidrosis"|"Degenerative skin disorders"|"Chronic ulcer of other specified sites"|"Other specified dermatoses"|"Decubitus ulcer, lower back"|"Sebaceous cyst"|"Vascular disorders of skin"|"Other dermatoses"|"Decubitus ulcer, hip"|"Other disorders of skin and subcutaneous tissue"|"Striae atrophicae"|"Other specified diseases of sebaceous glands"|"Ulcer of lower limbs, except pressure ulcer"|"Other specified hypertrophic and atrophic conditions of skin"|"Unspecified erythematous condition"|"Circumscribed scleroderma"|"Scar conditions and fibrosis of skin"|"Keratoderma, acquired"|"Secondary focal hyperhidrosis"</t>
+  </si>
+  <si>
+    <t>Rheumatoid_Arthritis_Related_Conditions</t>
+  </si>
+  <si>
+    <t>714.31|714.30|714.33|714.32|714|725.0|714.89|714.4|725|714.3|714.2|714.1|714.0|714.81|714.9|714.8</t>
+  </si>
+  <si>
+    <t>Polyarticular juvenile rheumatoid arthritis, acute|"Monoarticular juvenile rheumatoid arthritis"|"Rheumatoid arthritis"|"Felty's syndrome"|"Polyarticular juvenile rheumatoid arthritis, chronic or unspecified"|"Other specified inflammatory polyarthropathies"|"Unspecified inflammatory polyarthropathy"|"Rheumatoid lung"|"Polymyalgia rheumatica"|"Chronic postrheumatic arthropathy"|"Other rheumatoid arthritis with visceral or systemic involvement"|"Rheumatoid arthritis and other inflammatory polyarthropathies"|"Juvenile chronic polyarthritis"|"Pauciarticular juvenile rheumatoid arthritis"</t>
+  </si>
+  <si>
+    <t>Inflammatory_Spondylopathies</t>
+  </si>
+  <si>
+    <t>721.1|720.81|720.0|720.1|721.4|720.8|720.9|721.41|721.42|720|721.91|720.89</t>
+  </si>
+  <si>
+    <t>Spondylosis with myelopathy, lumbar region|"Ankylosing spondylitis and other inflammatory spondylopathies"|"Thoracic or lumbar spondylosis with myelopathy"|"Inflammatory spondylopathies in diseases classified elsewhere"|"Spondylosis of unspecified site with myelopathy"|"Spinal enthesopathy"|"Unspecified inflammatory spondylopathy"|"Cervical spondylosis with myelopathy"|"Spondylosis with myelopathy, thoracic region"|"Other inflammatory spondylopathies"|"Ankylosing spondylitis"</t>
+  </si>
 </sst>
 </file>
 
@@ -994,7 +1243,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
@@ -1013,6 +1262,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="185">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -51839,10 +52089,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -51858,7 +52108,7 @@
     <col min="9" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15">
+    <row r="1" spans="1:17" ht="15">
       <c r="A1" s="2" t="s">
         <v>77</v>
       </c>
@@ -51892,8 +52142,26 @@
       <c r="K1" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="15">
+      <c r="L1" t="s">
+        <v>223</v>
+      </c>
+      <c r="M1" t="s">
+        <v>224</v>
+      </c>
+      <c r="N1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O1" t="s">
+        <v>226</v>
+      </c>
+      <c r="P1" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
@@ -51908,7 +52176,7 @@
       </c>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:17">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -51923,7 +52191,7 @@
       </c>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:17">
       <c r="A4" s="2" t="s">
         <v>68</v>
       </c>
@@ -51938,7 +52206,7 @@
       </c>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:17">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
@@ -51953,7 +52221,7 @@
       </c>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:17">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -51968,7 +52236,7 @@
       </c>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:17">
       <c r="A7" s="2" t="s">
         <v>45</v>
       </c>
@@ -51983,7 +52251,7 @@
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:17">
       <c r="A8" s="2" t="s">
         <v>47</v>
       </c>
@@ -51998,7 +52266,7 @@
       </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:17" ht="15">
       <c r="A9" s="2" t="s">
         <v>55</v>
       </c>
@@ -52023,8 +52291,26 @@
       <c r="K9" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9" t="s">
+        <v>229</v>
+      </c>
+      <c r="M9" t="s">
+        <v>230</v>
+      </c>
+      <c r="N9" t="s">
+        <v>231</v>
+      </c>
+      <c r="O9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P9" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15">
       <c r="A10" s="2" t="s">
         <v>72</v>
       </c>
@@ -52049,8 +52335,26 @@
       <c r="K10" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="N10" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="O10" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="P10" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q10" s="16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15">
       <c r="A11" s="2" t="s">
         <v>74</v>
       </c>
@@ -52075,8 +52379,26 @@
       <c r="K11" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="M11" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="N11" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="O11" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="P11" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q11" s="16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15">
       <c r="A12" s="2" t="s">
         <v>62</v>
       </c>
@@ -52101,8 +52423,26 @@
       <c r="K12" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12" t="s">
+        <v>62</v>
+      </c>
+      <c r="M12" t="s">
+        <v>230</v>
+      </c>
+      <c r="N12" t="s">
+        <v>231</v>
+      </c>
+      <c r="O12" t="b">
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15">
       <c r="A13" s="2" t="s">
         <v>59</v>
       </c>
@@ -52127,8 +52467,26 @@
       <c r="K13" s="2" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="L13" t="s">
+        <v>240</v>
+      </c>
+      <c r="M13" t="s">
+        <v>241</v>
+      </c>
+      <c r="N13" t="s">
+        <v>231</v>
+      </c>
+      <c r="O13" t="b">
+        <v>0</v>
+      </c>
+      <c r="P13" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15">
       <c r="A14" s="2" t="s">
         <v>53</v>
       </c>
@@ -52153,8 +52511,26 @@
       <c r="K14" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="L14" t="s">
+        <v>244</v>
+      </c>
+      <c r="M14" t="s">
+        <v>245</v>
+      </c>
+      <c r="N14" t="s">
+        <v>231</v>
+      </c>
+      <c r="O14" t="b">
+        <v>0</v>
+      </c>
+      <c r="P14" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" s="2" t="s">
         <v>51</v>
       </c>
@@ -52169,7 +52545,7 @@
       </c>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:17">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
@@ -52184,7 +52560,7 @@
       </c>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:17">
       <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
@@ -52199,7 +52575,7 @@
       </c>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:17">
       <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
@@ -52214,7 +52590,7 @@
       </c>
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:17">
       <c r="A19" s="2" t="s">
         <v>41</v>
       </c>
@@ -52229,7 +52605,7 @@
       </c>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:17" ht="15">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
@@ -52254,8 +52630,26 @@
       <c r="K20" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="15">
+      <c r="L20" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="M20" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="N20" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="O20" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="P20" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q20" s="16" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="15">
       <c r="A21" s="2" t="s">
         <v>70</v>
       </c>
@@ -52280,8 +52674,26 @@
       <c r="K21" s="2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="15">
+      <c r="L21" t="s">
+        <v>252</v>
+      </c>
+      <c r="M21" t="s">
+        <v>249</v>
+      </c>
+      <c r="N21" t="s">
+        <v>231</v>
+      </c>
+      <c r="O21" t="b">
+        <v>0</v>
+      </c>
+      <c r="P21" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="15">
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
@@ -52306,8 +52718,26 @@
       <c r="K22" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="15">
+      <c r="L22" t="s">
+        <v>255</v>
+      </c>
+      <c r="M22" t="s">
+        <v>249</v>
+      </c>
+      <c r="N22" t="s">
+        <v>231</v>
+      </c>
+      <c r="O22" t="b">
+        <v>0</v>
+      </c>
+      <c r="P22" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="15">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -52332,8 +52762,26 @@
       <c r="K23" s="2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="15">
+      <c r="L23" t="s">
+        <v>258</v>
+      </c>
+      <c r="M23" t="s">
+        <v>249</v>
+      </c>
+      <c r="N23" t="s">
+        <v>231</v>
+      </c>
+      <c r="O23" t="b">
+        <v>0</v>
+      </c>
+      <c r="P23" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="15">
       <c r="A24" s="2" t="s">
         <v>9</v>
       </c>
@@ -52358,8 +52806,26 @@
       <c r="K24" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="15">
+      <c r="L24" t="s">
+        <v>261</v>
+      </c>
+      <c r="M24" t="s">
+        <v>249</v>
+      </c>
+      <c r="N24" t="s">
+        <v>231</v>
+      </c>
+      <c r="O24" t="b">
+        <v>0</v>
+      </c>
+      <c r="P24" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="15">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
@@ -52384,8 +52850,26 @@
       <c r="K25" s="2" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="15">
+      <c r="L25" t="s">
+        <v>264</v>
+      </c>
+      <c r="M25" t="s">
+        <v>249</v>
+      </c>
+      <c r="N25" t="s">
+        <v>231</v>
+      </c>
+      <c r="O25" t="b">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>446.1</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="15">
       <c r="A26" s="2" t="s">
         <v>66</v>
       </c>
@@ -52410,8 +52894,26 @@
       <c r="K26" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="15">
+      <c r="L26" t="s">
+        <v>66</v>
+      </c>
+      <c r="M26" t="s">
+        <v>249</v>
+      </c>
+      <c r="N26" t="s">
+        <v>231</v>
+      </c>
+      <c r="O26" t="b">
+        <v>0</v>
+      </c>
+      <c r="P26" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="15">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
@@ -52436,8 +52938,26 @@
       <c r="K27" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="L27" t="s">
+        <v>268</v>
+      </c>
+      <c r="M27" t="s">
+        <v>249</v>
+      </c>
+      <c r="N27" t="s">
+        <v>231</v>
+      </c>
+      <c r="O27" t="b">
+        <v>0</v>
+      </c>
+      <c r="P27" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="15">
       <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
@@ -52462,8 +52982,26 @@
       <c r="K28" s="2" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="15">
+      <c r="L28" t="s">
+        <v>271</v>
+      </c>
+      <c r="M28" t="s">
+        <v>249</v>
+      </c>
+      <c r="N28" t="s">
+        <v>231</v>
+      </c>
+      <c r="O28" t="b">
+        <v>0</v>
+      </c>
+      <c r="P28" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="15">
       <c r="A29" s="2" t="s">
         <v>17</v>
       </c>
@@ -52488,8 +53026,26 @@
       <c r="K29" s="2" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="15">
+      <c r="L29" t="s">
+        <v>274</v>
+      </c>
+      <c r="M29" t="s">
+        <v>275</v>
+      </c>
+      <c r="N29" t="s">
+        <v>231</v>
+      </c>
+      <c r="O29" t="b">
+        <v>0</v>
+      </c>
+      <c r="P29" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="15">
       <c r="A30" s="2" t="s">
         <v>31</v>
       </c>
@@ -52514,8 +53070,26 @@
       <c r="K30" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" ht="15">
+      <c r="L30" t="s">
+        <v>278</v>
+      </c>
+      <c r="M30" t="s">
+        <v>275</v>
+      </c>
+      <c r="N30" t="s">
+        <v>231</v>
+      </c>
+      <c r="O30" t="b">
+        <v>0</v>
+      </c>
+      <c r="P30" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="15">
       <c r="A31" s="2" t="s">
         <v>4</v>
       </c>
@@ -52540,8 +53114,26 @@
       <c r="K31" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="L31" t="s">
+        <v>281</v>
+      </c>
+      <c r="M31" t="s">
+        <v>249</v>
+      </c>
+      <c r="N31" t="s">
+        <v>231</v>
+      </c>
+      <c r="O31" t="b">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>579</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="15">
       <c r="A32" s="2" t="s">
         <v>19</v>
       </c>
@@ -52566,8 +53158,26 @@
       <c r="K32" s="2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" ht="15">
+      <c r="L32" t="s">
+        <v>282</v>
+      </c>
+      <c r="M32" t="s">
+        <v>249</v>
+      </c>
+      <c r="N32" t="s">
+        <v>231</v>
+      </c>
+      <c r="O32" t="b">
+        <v>0</v>
+      </c>
+      <c r="P32" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="15">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -52592,8 +53202,26 @@
       <c r="K33" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="15">
+      <c r="L33" t="s">
+        <v>285</v>
+      </c>
+      <c r="M33" t="s">
+        <v>249</v>
+      </c>
+      <c r="N33" t="s">
+        <v>231</v>
+      </c>
+      <c r="O33" t="b">
+        <v>0</v>
+      </c>
+      <c r="P33" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="15">
       <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
@@ -52618,8 +53246,26 @@
       <c r="K34" s="2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="35" spans="1:11">
+      <c r="L34" t="s">
+        <v>179</v>
+      </c>
+      <c r="M34" t="s">
+        <v>288</v>
+      </c>
+      <c r="N34" t="s">
+        <v>231</v>
+      </c>
+      <c r="O34" t="b">
+        <v>0</v>
+      </c>
+      <c r="P34" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="15">
       <c r="A35" s="2" t="s">
         <v>61</v>
       </c>
@@ -52644,8 +53290,26 @@
       <c r="K35" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" ht="15">
+      <c r="L35" t="s">
+        <v>291</v>
+      </c>
+      <c r="M35" t="s">
+        <v>288</v>
+      </c>
+      <c r="N35" t="s">
+        <v>231</v>
+      </c>
+      <c r="O35" t="b">
+        <v>0</v>
+      </c>
+      <c r="P35" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="15">
       <c r="A36" s="2" t="s">
         <v>2</v>
       </c>
@@ -52670,8 +53334,26 @@
       <c r="K36" s="2" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="37" spans="1:11">
+      <c r="L36" t="s">
+        <v>294</v>
+      </c>
+      <c r="M36" t="s">
+        <v>249</v>
+      </c>
+      <c r="N36" t="s">
+        <v>231</v>
+      </c>
+      <c r="O36" t="b">
+        <v>0</v>
+      </c>
+      <c r="P36" t="s">
+        <v>295</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="15">
       <c r="A37" s="2" t="s">
         <v>15</v>
       </c>
@@ -52696,8 +53378,26 @@
       <c r="K37" s="2" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" ht="15">
+      <c r="L37" s="16" t="s">
+        <v>297</v>
+      </c>
+      <c r="M37" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="N37" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="O37" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="P37" s="16" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q37" s="16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="15">
       <c r="A38" s="2" t="s">
         <v>11</v>
       </c>
@@ -52722,8 +53422,26 @@
       <c r="K38" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="1:11">
+      <c r="L38" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="M38" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="N38" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="O38" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="P38" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q38" s="16" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="15">
       <c r="A39" s="2" t="s">
         <v>21</v>
       </c>
@@ -52748,8 +53466,26 @@
       <c r="K39" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="40" spans="1:11">
+      <c r="L39" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="M39" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="N39" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="O39" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="P39" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q39" s="16" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="15">
       <c r="A40" s="2" t="s">
         <v>23</v>
       </c>
@@ -52773,6 +53509,24 @@
       </c>
       <c r="K40" s="2" t="s">
         <v>201</v>
+      </c>
+      <c r="L40" t="s">
+        <v>303</v>
+      </c>
+      <c r="M40" t="s">
+        <v>249</v>
+      </c>
+      <c r="N40" t="s">
+        <v>231</v>
+      </c>
+      <c r="O40" t="b">
+        <v>0</v>
+      </c>
+      <c r="P40" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>